<commit_message>
Change by Sathiya for Procedure.
</commit_message>
<xml_diff>
--- a/ExportToExcelNew.xlsx
+++ b/ExportToExcelNew.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="871" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="871" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Day1" sheetId="2" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="CurWeekBookingforNxtQTR" sheetId="15" r:id="rId9"/>
     <sheet name="TotalNextQTRShipment" sheetId="13" r:id="rId10"/>
     <sheet name="CurDateBooked4CurQtr" sheetId="16" r:id="rId11"/>
+    <sheet name="Procedure to Run" sheetId="17" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Current!$A$2:$J$23</definedName>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2364" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2365" uniqueCount="157">
   <si>
     <t xml:space="preserve">Sales Order </t>
   </si>
@@ -505,6 +506,9 @@
   </si>
   <si>
     <t>Q1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When you open this function from AX as Daily Order Update you get defaulted to Current date; if you leave that date and run. System will run for yesterday's </t>
   </si>
 </sst>
 </file>
@@ -995,6 +999,9 @@
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1015,9 +1022,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -5748,7 +5752,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:J2"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5905,6 +5909,29 @@
       </c>
       <c r="J5" s="24">
         <v>43025.503368055557</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B9:C9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -6952,10 +6979,10 @@
       <c r="I2" s="27"/>
       <c r="J2" s="27"/>
       <c r="K2" s="28"/>
-      <c r="M2" s="76" t="s">
+      <c r="M2" s="79" t="s">
         <v>27</v>
       </c>
-      <c r="N2" s="77"/>
+      <c r="N2" s="80"/>
       <c r="O2" s="36"/>
     </row>
     <row r="3" spans="2:15" ht="36" x14ac:dyDescent="0.25">
@@ -7206,22 +7233,22 @@
     </row>
     <row r="10" spans="2:15" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="2:15" ht="18.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B11" s="73" t="s">
+      <c r="B11" s="76" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="74"/>
-      <c r="D11" s="74"/>
-      <c r="E11" s="74"/>
-      <c r="F11" s="74"/>
-      <c r="G11" s="75"/>
-      <c r="I11" s="73" t="s">
+      <c r="C11" s="77"/>
+      <c r="D11" s="77"/>
+      <c r="E11" s="77"/>
+      <c r="F11" s="77"/>
+      <c r="G11" s="78"/>
+      <c r="I11" s="76" t="s">
         <v>137</v>
       </c>
-      <c r="J11" s="74"/>
-      <c r="K11" s="74"/>
-      <c r="L11" s="74"/>
-      <c r="M11" s="74"/>
-      <c r="N11" s="75"/>
+      <c r="J11" s="77"/>
+      <c r="K11" s="77"/>
+      <c r="L11" s="77"/>
+      <c r="M11" s="77"/>
+      <c r="N11" s="78"/>
       <c r="O11" s="37"/>
     </row>
     <row r="12" spans="2:15" ht="14.25" x14ac:dyDescent="0.25">
@@ -7424,7 +7451,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
@@ -7455,25 +7482,25 @@
       <c r="K1" s="5"/>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B2" s="83"/>
-      <c r="C2" s="83"/>
-      <c r="D2" s="83"/>
-      <c r="E2" s="83"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="83"/>
-      <c r="I2" s="85"/>
-      <c r="J2" s="85"/>
-      <c r="K2" s="85"/>
+      <c r="B2" s="73"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="75"/>
+      <c r="K2" s="75"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C4" s="79" t="s">
+      <c r="C4" s="82" t="s">
         <v>61</v>
       </c>
-      <c r="D4" s="80"/>
-      <c r="E4" s="80"/>
-      <c r="F4" s="80"/>
-      <c r="G4" s="80"/>
+      <c r="D4" s="83"/>
+      <c r="E4" s="83"/>
+      <c r="F4" s="83"/>
+      <c r="G4" s="83"/>
       <c r="H4" s="46"/>
       <c r="N4" s="47"/>
       <c r="O4" s="47" t="s">
@@ -7665,20 +7692,20 @@
       </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D13" s="78"/>
-      <c r="E13" s="78"/>
-      <c r="F13" s="78"/>
-      <c r="G13" s="78"/>
+      <c r="D13" s="81"/>
+      <c r="E13" s="81"/>
+      <c r="F13" s="81"/>
+      <c r="G13" s="81"/>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C15" s="79" t="s">
+      <c r="C15" s="82" t="s">
         <v>62</v>
       </c>
-      <c r="D15" s="80"/>
-      <c r="E15" s="80"/>
-      <c r="F15" s="80"/>
-      <c r="G15" s="80"/>
-      <c r="H15" s="82"/>
+      <c r="D15" s="83"/>
+      <c r="E15" s="83"/>
+      <c r="F15" s="83"/>
+      <c r="G15" s="83"/>
+      <c r="H15" s="85"/>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C16" s="43"/>
@@ -7864,10 +7891,10 @@
       <c r="C24" s="46"/>
       <c r="D24" s="46"/>
       <c r="E24" s="46"/>
-      <c r="F24" s="81" t="s">
+      <c r="F24" s="84" t="s">
         <v>60</v>
       </c>
-      <c r="G24" s="81"/>
+      <c r="G24" s="84"/>
       <c r="H24" s="46">
         <f>H22+H11</f>
         <v>448.61059999999998</v>

</xml_diff>

<commit_message>
second and third file added
</commit_message>
<xml_diff>
--- a/ExportToExcelNew.xlsx
+++ b/ExportToExcelNew.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\erptest2\InvResv\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\D365 Repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2365" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2366" uniqueCount="158">
   <si>
     <t xml:space="preserve">Sales Order </t>
   </si>
@@ -509,6 +509,9 @@
   </si>
   <si>
     <t xml:space="preserve">When you open this function from AX as Daily Order Update you get defaulted to Current date; if you leave that date and run. System will run for yesterday's </t>
+  </si>
+  <si>
+    <t>Don’t not change any formula in ProductTable</t>
   </si>
 </sst>
 </file>
@@ -5918,13 +5921,16 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B9:C9"/>
+  <dimension ref="B9:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="143.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9">
@@ -5932,6 +5938,14 @@
       </c>
       <c r="C9" t="s">
         <v>156</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>